<commit_message>
Update: Se Modifica Diagrama
</commit_message>
<xml_diff>
--- a/3- Desarrollo/04- Inventario Software Y Hardware/03- Sotfware_Kyukeisho.xlsx
+++ b/3- Desarrollo/04- Inventario Software Y Hardware/03- Sotfware_Kyukeisho.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APRENDIZ.DESKTOP-9L871TK\Pictures\sena_ceet\III TRIMESTRE\JAIRO VELASQUEZ\ESTIMADOS\HARDWARE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres\Proyecto_Formativo\Kyukeisho_New\3- Desarrollo\04- Inventario Software Y Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95648B91-62B6-4C79-88BC-7FAD3EC1ED52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BDEC43-42A5-4205-B9F2-27148F6C90D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -112,10 +113,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -128,67 +129,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -196,6 +138,29 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -224,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -366,105 +331,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,7 +454,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -727,437 +694,430 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:O21"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="212.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="6" max="6" width="212.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="1"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="1"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="35" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="5" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="G6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="H6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="I6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-    </row>
-    <row r="8" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
         <v>2</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="34" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="18" t="s">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="11">
+      <c r="G7" s="24">
         <v>1</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="H7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="I7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="24">
+      <c r="J7" s="26">
         <v>1199999</v>
       </c>
-      <c r="L8" s="24">
+      <c r="K7" s="26">
         <v>1199999</v>
       </c>
-      <c r="M8" s="24">
+      <c r="L7" s="26">
         <v>1199999</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>3</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="26" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="19" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="11">
+      <c r="G8" s="24">
         <v>1</v>
       </c>
-      <c r="I9" s="14">
+      <c r="H8" s="27">
         <v>21000</v>
       </c>
-      <c r="J9" s="44">
+      <c r="I8" s="28">
         <v>21000</v>
       </c>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="46"/>
-    </row>
-    <row r="10" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="29">
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>4</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="38" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="11">
+      <c r="G9" s="24">
         <v>1</v>
       </c>
-      <c r="I10" s="14">
+      <c r="H9" s="27">
         <v>59200</v>
       </c>
-      <c r="J10" s="24">
+      <c r="I9" s="26">
         <v>59200</v>
       </c>
-      <c r="K10" s="24">
+      <c r="J9" s="26">
         <v>59200</v>
       </c>
-      <c r="L10" s="24">
+      <c r="K9" s="26">
         <v>59200</v>
       </c>
-      <c r="M10" s="24">
+      <c r="L9" s="26">
         <v>59200</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="29">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
         <v>6</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="26" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="9" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="11">
+      <c r="G10" s="24">
         <v>1</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="29">
+      <c r="H10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
         <v>7</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="26" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="8" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="11">
+      <c r="G11" s="24">
         <v>1</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="24">
+      <c r="H11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="26">
         <v>2099099</v>
       </c>
-      <c r="L12" s="24">
+      <c r="K11" s="26">
         <v>2099099</v>
       </c>
-      <c r="M12" s="24">
+      <c r="L11" s="26">
         <v>2099099</v>
       </c>
-      <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="29">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
         <v>8</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="26" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="4" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="11">
+      <c r="G12" s="24">
         <v>1</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="21"/>
-    </row>
-    <row r="14" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="29">
+      <c r="H12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
         <v>9</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="41" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="6" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="11">
+      <c r="G13" s="24">
         <v>4</v>
       </c>
-      <c r="I14" s="16">
+      <c r="H13" s="31">
         <v>147612</v>
       </c>
-      <c r="J14" s="24">
-        <f>H14*I14</f>
+      <c r="I13" s="26">
+        <f>G13*H13</f>
         <v>590448</v>
       </c>
-      <c r="K14" s="24">
+      <c r="J13" s="26">
         <v>147612</v>
       </c>
-      <c r="L14" s="24">
+      <c r="K13" s="26">
         <v>147612</v>
       </c>
-      <c r="M14" s="24">
+      <c r="L13" s="26">
         <v>147612</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="39">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
         <v>10</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="42" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="12" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="13">
+      <c r="G14" s="35">
         <v>4</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="32" t="s">
+      <c r="H14" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="23">
-        <f>SUM(J8,J9,J10,J14)</f>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39">
+        <f>SUM(I7,I8,I9,I13)</f>
         <v>670648</v>
       </c>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-    </row>
-    <row r="17" spans="7:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G17" s="21"/>
-    </row>
-    <row r="19" spans="7:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K19" s="21"/>
-    </row>
-    <row r="21" spans="7:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I21" s="21"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="18" spans="8:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="20" spans="8:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B1:F5"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="31">
+    <mergeCell ref="F1:L5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>